<commit_message>
fix: split open and protected dataset and fix some cardinalities
</commit_message>
<xml_diff>
--- a/Formulasation(shacl)/core/Templates/SHACL-agent-open-protected.xlsx
+++ b/Formulasation(shacl)/core/Templates/SHACL-agent-open-protected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthri-my.sharepoint.com/personal/hannah_neikes_health-ri_nl/Documents/Documenten/GitHub/gdi-metadata/Formulasation(shacl)/core/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="275" documentId="13_ncr:1_{CC90F1A9-7F52-8148-BE94-617DCF70111C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58981EDD-3923-439C-B60A-59BBF885DD21}"/>
+  <xr:revisionPtr revIDLastSave="277" documentId="13_ncr:1_{CC90F1A9-7F52-8148-BE94-617DCF70111C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAABAA8E-9737-47C2-A02E-6575DF601C32}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-12765" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-12765" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prefixes" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="161">
   <si>
     <t>PREFIX</t>
   </si>
@@ -473,18 +473,6 @@
     <t>A type of organisation that makes the Dataset available</t>
   </si>
   <si>
-    <t>healthdcatap:trustedDataHolder</t>
-  </si>
-  <si>
-    <t>trusted data holder</t>
-  </si>
-  <si>
-    <t>A data holder that has been designated by the Member State to facilitate direct data sharing.</t>
-  </si>
-  <si>
-    <t>xsd:boolean</t>
-  </si>
-  <si>
     <t>gdi</t>
   </si>
   <si>
@@ -522,15 +510,6 @@
   </si>
   <si>
     <t>A name of the agent.</t>
-  </si>
-  <si>
-    <t>dct:type</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>A type of the agent that makes the Catalogue or Dataset available</t>
   </si>
   <si>
     <t>foaf:homepage</t>
@@ -1316,7 +1295,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1474,9 +1453,6 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="49" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="49" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
@@ -2215,10 +2191,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2255,7 +2231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
+    <sheetView zoomScale="95" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="B13" sqref="B13"/>
       <selection pane="topRight" activeCell="B5" sqref="B5"/>
@@ -2283,7 +2259,7 @@
         <v>43</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F1" s="3"/>
     </row>
@@ -2301,7 +2277,7 @@
         <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F3" s="3"/>
     </row>
@@ -2310,7 +2286,7 @@
         <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="F4" s="3"/>
     </row>
@@ -2319,7 +2295,7 @@
         <v>48</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -2449,10 +2425,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>79</v>
@@ -2492,12 +2468,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Y27"/>
+  <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView zoomScale="95" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="E13" sqref="E13"/>
-      <selection pane="topRight" activeCell="F27" sqref="F27"/>
+      <selection pane="topRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2505,10 +2481,10 @@
     <col min="1" max="1" width="46" style="48" customWidth="1"/>
     <col min="2" max="2" width="41.44140625" style="49" customWidth="1"/>
     <col min="3" max="3" width="42.6640625" style="48" customWidth="1"/>
-    <col min="4" max="4" width="26.88671875" style="64" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" style="63" customWidth="1"/>
     <col min="5" max="5" width="41.44140625" style="49" customWidth="1"/>
     <col min="6" max="6" width="41.109375" style="45" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" style="65" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="64" customWidth="1"/>
     <col min="8" max="8" width="12" style="46" customWidth="1"/>
     <col min="9" max="9" width="20.109375" style="48" customWidth="1"/>
     <col min="10" max="11" width="21" style="48" customWidth="1"/>
@@ -2529,195 +2505,195 @@
       <c r="A1" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="63" t="s">
-        <v>149</v>
+      <c r="B1" s="62" t="s">
+        <v>145</v>
       </c>
       <c r="C1" s="49"/>
       <c r="P1" s="49"/>
       <c r="S1" s="49"/>
     </row>
-    <row r="3" spans="1:25" s="68" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="66" t="s">
+    <row r="3" spans="1:25" s="67" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="D3" s="69"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="Q3" s="72"/>
-      <c r="R3" s="72"/>
-      <c r="T3" s="72"/>
-      <c r="U3" s="72"/>
-      <c r="V3" s="72"/>
-      <c r="W3" s="72"/>
+      <c r="B3" s="66"/>
+      <c r="D3" s="68"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="Q3" s="71"/>
+      <c r="R3" s="71"/>
+      <c r="T3" s="71"/>
+      <c r="U3" s="71"/>
+      <c r="V3" s="71"/>
+      <c r="W3" s="71"/>
     </row>
     <row r="4" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="73"/>
-      <c r="G4" s="74"/>
+      <c r="D4" s="72"/>
+      <c r="G4" s="73"/>
       <c r="Q4" s="49"/>
     </row>
-    <row r="5" spans="1:25" s="75" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="75" t="s">
+    <row r="5" spans="1:25" s="74" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="74" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="76" t="s">
+      <c r="D5" s="75" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="75" t="s">
+      <c r="E5" s="74" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="77" t="s">
+      <c r="F5" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="G5" s="78" t="s">
+      <c r="G5" s="77" t="s">
         <v>88</v>
       </c>
-      <c r="H5" s="78" t="s">
+      <c r="H5" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="I5" s="75" t="s">
+      <c r="I5" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="J5" s="75" t="s">
+      <c r="J5" s="74" t="s">
         <v>91</v>
       </c>
-      <c r="K5" s="75" t="s">
+      <c r="K5" s="74" t="s">
         <v>92</v>
       </c>
-      <c r="L5" s="75" t="s">
+      <c r="L5" s="74" t="s">
         <v>93</v>
       </c>
-      <c r="M5" s="75" t="s">
+      <c r="M5" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="N5" s="75" t="s">
+      <c r="N5" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="O5" s="75" t="s">
+      <c r="O5" s="74" t="s">
         <v>96</v>
       </c>
-      <c r="P5" s="75" t="s">
+      <c r="P5" s="74" t="s">
         <v>97</v>
       </c>
-      <c r="Q5" s="75" t="s">
+      <c r="Q5" s="74" t="s">
         <v>98</v>
       </c>
-      <c r="R5" s="75" t="s">
+      <c r="R5" s="74" t="s">
         <v>99</v>
       </c>
-      <c r="S5" s="75" t="s">
+      <c r="S5" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="T5" s="75" t="s">
+      <c r="T5" s="74" t="s">
         <v>101</v>
       </c>
-      <c r="U5" s="75" t="s">
+      <c r="U5" s="74" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:25" s="79" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A6" s="79" t="s">
+    <row r="6" spans="1:25" s="78" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="78" t="s">
         <v>103</v>
       </c>
-      <c r="B6" s="79" t="s">
+      <c r="B6" s="78" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="79" t="s">
+      <c r="C6" s="78" t="s">
         <v>105</v>
       </c>
-      <c r="D6" s="80" t="s">
+      <c r="D6" s="79" t="s">
         <v>106</v>
       </c>
-      <c r="E6" s="79" t="s">
+      <c r="E6" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="F6" s="81" t="s">
+      <c r="F6" s="80" t="s">
         <v>108</v>
       </c>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="81"/>
     </row>
     <row r="7" spans="1:25" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="83" t="s">
+      <c r="A7" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="83" t="s">
         <v>109</v>
       </c>
-      <c r="C7" s="83" t="s">
+      <c r="C7" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="D7" s="85" t="s">
+      <c r="D7" s="84" t="s">
         <v>111</v>
       </c>
-      <c r="E7" s="83" t="s">
+      <c r="E7" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="F7" s="86" t="s">
+      <c r="F7" s="85" t="s">
         <v>113</v>
       </c>
-      <c r="G7" s="87" t="s">
+      <c r="G7" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="H7" s="87" t="s">
+      <c r="H7" s="86" t="s">
         <v>115</v>
       </c>
-      <c r="I7" s="84" t="s">
+      <c r="I7" s="83" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="84" t="s">
+      <c r="J7" s="83" t="s">
         <v>116</v>
       </c>
-      <c r="K7" s="88" t="s">
+      <c r="K7" s="87" t="s">
         <v>117</v>
       </c>
-      <c r="L7" s="89" t="s">
+      <c r="L7" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="M7" s="84" t="s">
+      <c r="M7" s="83" t="s">
         <v>119</v>
       </c>
-      <c r="N7" s="84" t="s">
+      <c r="N7" s="83" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="84" t="s">
+      <c r="O7" s="83" t="s">
         <v>121</v>
       </c>
-      <c r="P7" s="88" t="s">
+      <c r="P7" s="87" t="s">
         <v>122</v>
       </c>
-      <c r="Q7" s="89" t="s">
+      <c r="Q7" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="R7" s="84" t="s">
+      <c r="R7" s="83" t="s">
         <v>123</v>
       </c>
-      <c r="S7" s="84" t="s">
+      <c r="S7" s="83" t="s">
         <v>124</v>
       </c>
-      <c r="T7" s="84" t="s">
+      <c r="T7" s="83" t="s">
         <v>125</v>
       </c>
-      <c r="U7" s="84" t="s">
+      <c r="U7" s="83" t="s">
         <v>123</v>
       </c>
-      <c r="V7" s="84" t="s">
+      <c r="V7" s="83" t="s">
         <v>126</v>
       </c>
-      <c r="W7" s="84" t="s">
+      <c r="W7" s="83" t="s">
         <v>127</v>
       </c>
-      <c r="X7" s="84" t="s">
+      <c r="X7" s="83" t="s">
         <v>128</v>
       </c>
-      <c r="Y7" s="84" t="s">
+      <c r="Y7" s="83" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2737,20 +2713,20 @@
     </row>
     <row r="9" spans="1:25" ht="72" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="str">
-        <f t="shared" ref="A9:A12" si="0">CONCATENATE(B9,"#",C9)</f>
+        <f t="shared" ref="A9:A11" si="0">CONCATENATE(B9,"#",C9)</f>
         <v>gdi:AgentOpenProtectedShape#foaf:mbox</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D9" s="43" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G9" s="32">
         <v>1</v>
@@ -2763,7 +2739,7 @@
       </c>
       <c r="K9" s="33"/>
       <c r="V9" s="49" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="X9" s="50" t="s">
         <v>132</v>
@@ -2778,16 +2754,16 @@
         <v>gdi:AgentOpenProtectedShape#foaf:name</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C10" s="51" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F10" s="54"/>
       <c r="G10" s="40">
@@ -2810,200 +2786,159 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="str">
-        <f t="shared" si="0"/>
-        <v>gdi:AgentOpenProtectedShape#dct:type</v>
-      </c>
-      <c r="B11" s="49" t="s">
-        <v>152</v>
-      </c>
-      <c r="C11" s="60" t="s">
-        <v>160</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="E11" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="G11" s="32"/>
-      <c r="H11" s="46">
-        <v>1</v>
-      </c>
-      <c r="I11" s="50" t="s">
-        <v>131</v>
-      </c>
-      <c r="K11" s="33"/>
-      <c r="X11" s="50" t="s">
-        <v>132</v>
-      </c>
-      <c r="Y11" s="50" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="57" t="str">
+    <row r="11" spans="1:25" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="57" t="str">
         <f t="shared" si="0"/>
         <v>gdi:AgentOpenProtectedShape#foaf:homepage</v>
       </c>
-      <c r="B12" s="58" t="s">
-        <v>152</v>
-      </c>
-      <c r="C12" s="51" t="s">
-        <v>163</v>
-      </c>
-      <c r="D12" s="61" t="s">
-        <v>164</v>
-      </c>
-      <c r="E12" s="62" t="s">
-        <v>165</v>
-      </c>
-      <c r="F12" s="54"/>
-      <c r="G12" s="40">
+      <c r="B11" s="58" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="D11" s="60" t="s">
+        <v>157</v>
+      </c>
+      <c r="E11" s="61" t="s">
+        <v>158</v>
+      </c>
+      <c r="F11" s="54"/>
+      <c r="G11" s="40">
         <v>1</v>
       </c>
-      <c r="H12" s="55">
+      <c r="H11" s="55">
         <v>1</v>
       </c>
-      <c r="I12" s="59" t="s">
+      <c r="I11" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="J12" s="57"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="57"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="57"/>
-      <c r="P12" s="57"/>
-      <c r="Q12" s="57"/>
-      <c r="R12" s="57"/>
-      <c r="S12" s="57"/>
-      <c r="T12" s="58"/>
-      <c r="U12" s="58"/>
-      <c r="V12" s="58"/>
-      <c r="W12" s="58"/>
-      <c r="X12" s="59" t="s">
+      <c r="J11" s="57"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="57"/>
+      <c r="S11" s="57"/>
+      <c r="T11" s="58"/>
+      <c r="U11" s="58"/>
+      <c r="V11" s="58"/>
+      <c r="W11" s="58"/>
+      <c r="X11" s="59" t="s">
         <v>132</v>
       </c>
-      <c r="Y12" s="59" t="s">
+      <c r="Y11" s="59" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A13" s="48" t="str">
-        <f>CONCATENATE(B13,"#",C13)</f>
+    <row r="12" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="48" t="str">
+        <f>CONCATENATE(B12,"#",C12)</f>
         <v>gdi:AgentOpenProtectedShape#healthdcatap:publishernote</v>
       </c>
-      <c r="B13" s="90" t="s">
-        <v>152</v>
-      </c>
-      <c r="C13" s="31" t="s">
+      <c r="B12" s="89" t="s">
+        <v>148</v>
+      </c>
+      <c r="C12" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="D13" s="91" t="s">
+      <c r="D12" s="90" t="s">
         <v>138</v>
       </c>
-      <c r="E13" s="92" t="s">
+      <c r="E12" s="91" t="s">
         <v>139</v>
       </c>
-      <c r="G13" s="32"/>
-      <c r="H13" s="46">
+      <c r="G12" s="32"/>
+      <c r="H12" s="46">
         <v>1</v>
       </c>
-      <c r="I13" s="47" t="s">
+      <c r="I12" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="X12" s="50"/>
+      <c r="Y12" s="50"/>
+    </row>
+    <row r="13" spans="1:25" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="57" t="str">
+        <f t="shared" ref="A13" si="1">CONCATENATE(B13,"#",C13)</f>
+        <v>gdi:AgentOpenProtectedShape#healthdcatap:publishertype</v>
+      </c>
+      <c r="B13" s="92" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13" s="93" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" s="94" t="s">
+        <v>142</v>
+      </c>
+      <c r="F13" s="54"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="55">
+        <v>1</v>
+      </c>
+      <c r="I13" s="59" t="s">
+        <v>131</v>
+      </c>
+      <c r="J13" s="57"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="57"/>
+      <c r="P13" s="57"/>
+      <c r="Q13" s="57"/>
+      <c r="R13" s="57"/>
+      <c r="S13" s="57"/>
+      <c r="T13" s="58"/>
+      <c r="U13" s="58"/>
+      <c r="V13" s="58"/>
+      <c r="W13" s="58"/>
       <c r="X13" s="50"/>
       <c r="Y13" s="50"/>
     </row>
-    <row r="14" spans="1:25" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="57" t="str">
-        <f t="shared" ref="A14:A15" si="1">CONCATENATE(B14,"#",C14)</f>
-        <v>gdi:AgentOpenProtectedShape#healthdcatap:publishertype</v>
-      </c>
-      <c r="B14" s="93" t="s">
-        <v>152</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="D14" s="94" t="s">
-        <v>141</v>
-      </c>
-      <c r="E14" s="95" t="s">
-        <v>142</v>
-      </c>
-      <c r="F14" s="54"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="55">
-        <v>1</v>
-      </c>
-      <c r="I14" s="59" t="s">
-        <v>131</v>
-      </c>
-      <c r="J14" s="57"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="57"/>
-      <c r="M14" s="57"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="57"/>
-      <c r="P14" s="57"/>
-      <c r="Q14" s="57"/>
-      <c r="R14" s="57"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="58"/>
-      <c r="U14" s="58"/>
-      <c r="V14" s="58"/>
-      <c r="W14" s="58"/>
+    <row r="14" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B14" s="89"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="36"/>
+      <c r="G14" s="32"/>
+      <c r="I14" s="47"/>
+      <c r="L14" s="33"/>
       <c r="X14" s="50"/>
       <c r="Y14" s="50"/>
     </row>
-    <row r="15" spans="1:25" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A15" s="48" t="str">
-        <f t="shared" si="1"/>
-        <v>gdi:AgentOpenProtectedShape#healthdcatap:trustedDataHolder</v>
-      </c>
-      <c r="B15" s="90" t="s">
-        <v>152</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="E15" s="49" t="s">
-        <v>145</v>
-      </c>
+    <row r="15" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B15" s="89"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="37"/>
       <c r="G15" s="32"/>
-      <c r="H15" s="46">
-        <v>1</v>
-      </c>
-      <c r="I15" s="47" t="s">
-        <v>134</v>
-      </c>
-      <c r="J15" s="47" t="s">
-        <v>146</v>
-      </c>
+      <c r="I15" s="47"/>
+      <c r="K15" s="33"/>
       <c r="X15" s="50"/>
       <c r="Y15" s="50"/>
     </row>
     <row r="16" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B16" s="90"/>
-      <c r="C16" s="35"/>
+      <c r="B16" s="89"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="36"/>
+      <c r="E16" s="38"/>
       <c r="G16" s="32"/>
-      <c r="I16" s="47"/>
-      <c r="L16" s="33"/>
+      <c r="J16" s="33"/>
       <c r="X16" s="50"/>
       <c r="Y16" s="50"/>
     </row>
     <row r="17" spans="2:25" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B17" s="90"/>
+      <c r="B17" s="89"/>
       <c r="C17" s="34"/>
       <c r="D17" s="34"/>
       <c r="E17" s="37"/>
@@ -3014,88 +2949,67 @@
       <c r="Y17" s="50"/>
     </row>
     <row r="18" spans="2:25" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B18" s="90"/>
+      <c r="B18" s="89"/>
       <c r="C18" s="34"/>
       <c r="D18" s="34"/>
       <c r="E18" s="38"/>
       <c r="G18" s="32"/>
       <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
       <c r="X18" s="50"/>
       <c r="Y18" s="50"/>
     </row>
     <row r="19" spans="2:25" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B19" s="90"/>
+      <c r="B19" s="89"/>
       <c r="C19" s="34"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="37"/>
+      <c r="E19" s="39"/>
       <c r="G19" s="32"/>
-      <c r="I19" s="47"/>
-      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
       <c r="X19" s="50"/>
       <c r="Y19" s="50"/>
     </row>
     <row r="20" spans="2:25" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B20" s="90"/>
-      <c r="C20" s="34"/>
+      <c r="B20" s="89"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="38"/>
+      <c r="E20" s="35"/>
       <c r="G20" s="32"/>
-      <c r="J20" s="33"/>
+      <c r="I20" s="50"/>
       <c r="K20" s="33"/>
-      <c r="X20" s="50"/>
-      <c r="Y20" s="50"/>
     </row>
     <row r="21" spans="2:25" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B21" s="90"/>
+      <c r="B21" s="89"/>
       <c r="C21" s="34"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="39"/>
+      <c r="E21" s="38"/>
       <c r="G21" s="32"/>
-      <c r="L21" s="33"/>
-      <c r="X21" s="50"/>
-      <c r="Y21" s="50"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="33"/>
     </row>
     <row r="22" spans="2:25" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B22" s="90"/>
-      <c r="C22" s="35"/>
+      <c r="B22" s="89"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="35"/>
+      <c r="E22" s="38"/>
       <c r="G22" s="32"/>
-      <c r="I22" s="50"/>
-      <c r="K22" s="33"/>
+      <c r="J22" s="33"/>
     </row>
     <row r="23" spans="2:25" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B23" s="90"/>
-      <c r="C23" s="34"/>
+      <c r="B23" s="89"/>
       <c r="D23" s="34"/>
       <c r="E23" s="38"/>
       <c r="G23" s="32"/>
       <c r="I23" s="50"/>
-      <c r="J23" s="33"/>
-    </row>
-    <row r="24" spans="2:25" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B24" s="90"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="38"/>
-      <c r="G24" s="32"/>
-      <c r="J24" s="33"/>
-    </row>
-    <row r="25" spans="2:25" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B25" s="90"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="38"/>
-      <c r="G25" s="32"/>
-      <c r="I25" s="50"/>
-      <c r="K25" s="33"/>
-    </row>
-    <row r="26" spans="2:25" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B26" s="90"/>
-    </row>
-    <row r="27" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="90"/>
+      <c r="K23" s="33"/>
+    </row>
+    <row r="24" spans="2:25" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B24" s="89"/>
+    </row>
+    <row r="25" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="89"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G9:G25">
+  <conditionalFormatting sqref="G9:G23">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>"reviewd"</formula>
     </cfRule>
@@ -3104,7 +3018,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G25 G9:G23" xr:uid="{EDC952CC-97B4-994F-AA14-28A44C65C7A2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G23 G9:G21" xr:uid="{EDC952CC-97B4-994F-AA14-28A44C65C7A2}">
       <formula1>"0..n, 0..1, 1, 1..n"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3145,27 +3059,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
-    <Categorie xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
-    <Persoon xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Persoon>
-    <Opmerkingen xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B1A1CF98C819F4881BB4349588D0C85" ma:contentTypeVersion="22" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31f6c59cfd598d1d7de5b45c1822abcd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cfc87205-1831-4b6c-a7b4-76d40079a43e" xmlns:ns3="221af607-abea-4d5e-830c-567dcc03c0ec" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="67714481eaab3d0eef8b708c465ce66d" ns2:_="" ns3:_="">
     <xsd:import namespace="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
@@ -3453,6 +3346,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
+    <Categorie xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
+    <Persoon xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Persoon>
+    <Opmerkingen xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CE3AE30-F94D-4B2D-A964-81B3B3999808}">
   <ds:schemaRefs>
@@ -3462,17 +3376,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6C2A762-C9A0-490C-9DDC-F35C0AECA17E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
-    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1961BA38-9B45-4614-9139-CECC3763978C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3489,4 +3392,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6C2A762-C9A0-490C-9DDC-F35C0AECA17E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
+    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>